<commit_message>
Fix Biome temperature not available
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/block_temperature.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/block_temperature.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t/>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>crockpot:portable_crock_pot</t>
+  </si>
+  <si>
+    <t>charcoal_pit:log_pile</t>
   </si>
 </sst>
 </file>
@@ -522,7 +525,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr/>
-  <dimension ref="F44"/>
+  <dimension ref="F45"/>
   <sheetViews>
     <sheetView showGridLines="true" tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -1283,6 +1286,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="6">
+        <v>300</v>
+      </c>
+      <c r="C45" s="6">
+        <v>3</v>
+      </c>
+      <c r="D45" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Optimize wet-wind mechanics for feeling temperature - Humidity and wind are now accounted in feel temp, directly visible in orb - They also now contribute more directly to heat exchange process, but exact rates may need tweaking.
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/block_temperature.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/block_temperature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497922A8-46F8-8E44-9B7C-AB1D0753B580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B078D1-8361-D349-BF72-A6486E989556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -222,9 +222,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" zoomScale="288" zoomScaleNormal="288" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -554,7 +554,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
@@ -571,7 +571,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -622,10 +622,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="C7" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="b">
         <v>0</v>
@@ -639,10 +639,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="1">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1" t="b">
         <v>0</v>
@@ -656,7 +656,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="1">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="C9" s="1">
         <v>5</v>
@@ -792,7 +792,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="1">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="C17" s="1">
         <v>4</v>
@@ -809,7 +809,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="1">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="C18" s="1">
         <v>4</v>
@@ -826,7 +826,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="1">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="C19" s="1">
         <v>4</v>
@@ -843,7 +843,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="1">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="C20" s="1">
         <v>4</v>
@@ -860,7 +860,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="1">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="C21" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
may fix thermos dupe
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/block_temperature.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/block_temperature.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\eclipse-workspace\frostedheart-newdev\src\datagen\resources\data\frostedheart\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B38D270-F6CF-1C4D-854A-E74249E64140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91416170-552C-4D34-842E-9BDD0C62C08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="block_temperature" sheetId="1" r:id="rId1"/>
@@ -170,7 +170,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +193,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -237,10 +243,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -515,20 +521,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="288" zoomScaleNormal="288" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScale="288" zoomScaleNormal="288" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="33.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="3" customWidth="1"/>
     <col min="3" max="3" width="9" style="3"/>
     <col min="4" max="4" width="10.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -562,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -579,12 +585,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -596,7 +602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -613,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -630,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -647,7 +653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -664,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -681,7 +687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -698,7 +704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -715,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -732,7 +738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -749,7 +755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -766,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -783,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -800,7 +806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -817,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -834,7 +840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -851,7 +857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -868,7 +874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -885,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -902,7 +908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.25" customHeight="1">
+    <row r="23" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -919,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -936,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.25" customHeight="1">
+    <row r="25" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -953,7 +959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.25" customHeight="1">
+    <row r="26" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -970,7 +976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.25" customHeight="1">
+    <row r="27" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
@@ -987,7 +993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.25" customHeight="1">
+    <row r="28" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -1004,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.25" customHeight="1">
+    <row r="29" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -1038,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.25" customHeight="1">
+    <row r="31" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.25" customHeight="1">
+    <row r="32" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
@@ -1072,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.25" customHeight="1">
+    <row r="33" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1089,7 +1095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.25" customHeight="1">
+    <row r="34" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>37</v>
       </c>
@@ -1106,7 +1112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.25" customHeight="1">
+    <row r="35" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>38</v>
       </c>
@@ -1123,7 +1129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.25" customHeight="1">
+    <row r="36" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>39</v>
       </c>
@@ -1140,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -1157,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
@@ -1174,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
@@ -1191,7 +1197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.25" customHeight="1">
+    <row r="41" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>44</v>
       </c>
@@ -1225,7 +1231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.25" customHeight="1">
+    <row r="42" spans="1:5" ht="15.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>45</v>
       </c>
@@ -1242,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>47</v>
       </c>
@@ -1277,6 +1283,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>